<commit_message>
Atualizar código com melhorias
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -35,15 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">eu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/8/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/8/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/8/2025</t>
   </si>
 </sst>
 </file>
@@ -52,7 +43,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -123,7 +114,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,7 +244,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,8 +276,8 @@
       <c r="B2" s="0" t="n">
         <v>5541998217975</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="1" t="n">
+        <v>45899</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,8 +287,8 @@
       <c r="B3" s="0" t="n">
         <v>5541998217975</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+      <c r="C3" s="1" t="n">
+        <v>45889</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,8 +298,8 @@
       <c r="B4" s="0" t="n">
         <v>5541998217975</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="1" t="n">
+        <v>45879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>